<commit_message>
Modify scripts about DeviceConfig.xml
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/Keywordscripts/400.30.10_ApplicationImportManagedDeviceFromG1.xlsx
+++ b/NformTester/NformTester/Keywordscripts/400.30.10_ApplicationImportManagedDeviceFromG1.xlsx
@@ -3661,10 +3661,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>$SNMP_GXT_0_NAME$</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>"Description for GXT"</t>
   </si>
   <si>
@@ -3777,6 +3773,10 @@
   </si>
   <si>
     <t>;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$NAME_SNMP_GXT_0$</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4760,8 +4760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="D40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I65" sqref="I65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4834,7 +4834,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="E2" s="24"/>
       <c r="F2" s="24"/>
@@ -4919,7 +4919,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>191</v>
@@ -4964,16 +4964,16 @@
         <v>806</v>
       </c>
       <c r="J6" s="18" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="K6" s="18" t="s">
+        <v>807</v>
+      </c>
+      <c r="L6" s="18" t="s">
         <v>808</v>
       </c>
-      <c r="L6" s="18" t="s">
+      <c r="M6" s="18" t="s">
         <v>809</v>
-      </c>
-      <c r="M6" s="18" t="s">
-        <v>810</v>
       </c>
       <c r="N6" s="20"/>
       <c r="O6" s="21"/>
@@ -4989,7 +4989,7 @@
         <v>6</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>800</v>
@@ -5029,19 +5029,19 @@
         <v>805</v>
       </c>
       <c r="I8" s="18" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="J8" s="18" t="s">
+        <v>838</v>
+      </c>
+      <c r="K8" s="18" t="s">
         <v>807</v>
       </c>
-      <c r="K8" s="18" t="s">
+      <c r="L8" s="18" t="s">
         <v>808</v>
       </c>
-      <c r="L8" s="18" t="s">
+      <c r="M8" s="18" t="s">
         <v>809</v>
-      </c>
-      <c r="M8" s="18" t="s">
-        <v>810</v>
       </c>
       <c r="N8" s="20"/>
       <c r="O8" s="11"/>
@@ -5057,7 +5057,7 @@
         <v>8</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -5235,7 +5235,7 @@
         <v>4</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="I15" s="18"/>
       <c r="J15" s="18"/>
@@ -5425,7 +5425,7 @@
         <v>796</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>312</v>
@@ -5470,7 +5470,7 @@
         <v>23</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="E24" s="14" t="s">
         <v>728</v>
@@ -5524,7 +5524,7 @@
         <v>25</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>191</v>
@@ -5549,7 +5549,7 @@
         <v>26</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E27" s="14"/>
       <c r="F27" s="4"/>
@@ -5627,7 +5627,7 @@
         <v>573</v>
       </c>
       <c r="G30" s="18" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="H30" s="18">
         <v>3</v>
@@ -5684,13 +5684,13 @@
         <v>7</v>
       </c>
       <c r="H32" s="14" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="I32" s="18" t="s">
         <v>798</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
@@ -5753,18 +5753,18 @@
         <v>34</v>
       </c>
       <c r="D35" s="19" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="F35" s="18"/>
       <c r="G35" s="18"/>
       <c r="H35" s="18" t="s">
+        <v>833</v>
+      </c>
+      <c r="I35" s="18" t="s">
         <v>834</v>
-      </c>
-      <c r="I35" s="18" t="s">
-        <v>835</v>
       </c>
       <c r="J35" s="18" t="b">
         <v>1</v>
@@ -5849,10 +5849,10 @@
         <v>38</v>
       </c>
       <c r="D39" s="19" t="s">
+        <v>820</v>
+      </c>
+      <c r="E39" s="14" t="s">
         <v>821</v>
-      </c>
-      <c r="E39" s="14" t="s">
-        <v>822</v>
       </c>
       <c r="F39" s="18" t="s">
         <v>573</v>
@@ -5861,7 +5861,7 @@
         <v>3</v>
       </c>
       <c r="H39" s="18" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
@@ -5876,10 +5876,10 @@
         <v>39</v>
       </c>
       <c r="D40" s="19" t="s">
+        <v>820</v>
+      </c>
+      <c r="E40" s="14" t="s">
         <v>821</v>
-      </c>
-      <c r="E40" s="14" t="s">
-        <v>822</v>
       </c>
       <c r="F40" s="18" t="s">
         <v>178</v>
@@ -5901,7 +5901,7 @@
         <v>40</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="E41" s="18" t="s">
         <v>578</v>
@@ -5926,7 +5926,7 @@
         <v>41</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="E42" s="18" t="s">
         <v>800</v>
@@ -5949,10 +5949,10 @@
         <v>42</v>
       </c>
       <c r="D43" s="19" t="s">
+        <v>820</v>
+      </c>
+      <c r="E43" s="14" t="s">
         <v>821</v>
-      </c>
-      <c r="E43" s="14" t="s">
-        <v>822</v>
       </c>
       <c r="F43" s="18" t="s">
         <v>95</v>
@@ -6024,7 +6024,7 @@
         <v>45</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="E46" s="14" t="s">
         <v>300</v>
@@ -6036,7 +6036,7 @@
         <v>56</v>
       </c>
       <c r="H46" s="14" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
@@ -6051,7 +6051,7 @@
         <v>46</v>
       </c>
       <c r="D47" s="13" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="E47" s="14" t="s">
         <v>300</v>
@@ -6076,7 +6076,7 @@
         <v>47</v>
       </c>
       <c r="D48" s="13" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="E48" s="14" t="s">
         <v>300</v>
@@ -6163,7 +6163,7 @@
         <v>56</v>
       </c>
       <c r="H51" s="14" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="I51" s="4"/>
       <c r="J51" s="4"/>
@@ -6240,7 +6240,7 @@
         <v>56</v>
       </c>
       <c r="H54" s="14" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="I54" s="4"/>
       <c r="J54" s="4"/>
@@ -6317,7 +6317,7 @@
         <v>56</v>
       </c>
       <c r="H57" s="14" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="I57" s="4"/>
       <c r="J57" s="4"/>
@@ -6438,7 +6438,7 @@
         <v>19</v>
       </c>
       <c r="F62" s="18" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="G62" s="18" t="s">
         <v>2</v>
@@ -6469,7 +6469,7 @@
         <v>56</v>
       </c>
       <c r="H63" s="14" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="I63" s="4"/>
       <c r="J63" s="4"/>
@@ -6584,7 +6584,7 @@
         <v>67</v>
       </c>
       <c r="D68" s="13" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="E68" s="14" t="s">
         <v>392</v>
@@ -6609,7 +6609,7 @@
         <v>68</v>
       </c>
       <c r="D69" s="13" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="E69" s="14" t="s">
         <v>392</v>
@@ -6621,7 +6621,7 @@
         <v>3</v>
       </c>
       <c r="H69" s="18" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="I69" s="4"/>
       <c r="J69" s="4"/>
@@ -6636,7 +6636,7 @@
         <v>69</v>
       </c>
       <c r="D70" s="13" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="E70" s="14" t="s">
         <v>392</v>
@@ -6661,7 +6661,7 @@
         <v>70</v>
       </c>
       <c r="D71" s="13" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="E71" s="14" t="s">
         <v>392</v>
@@ -6673,7 +6673,7 @@
         <v>4</v>
       </c>
       <c r="H71" s="14" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="I71" s="4"/>
       <c r="J71" s="4"/>
@@ -6688,7 +6688,7 @@
         <v>71</v>
       </c>
       <c r="D72" s="13" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="E72" s="14" t="s">
         <v>392</v>

</xml_diff>